<commit_message>
arreglando el excel y los certificados RTC
</commit_message>
<xml_diff>
--- a/produccion/certificadosexcel.xlsx
+++ b/produccion/certificadosexcel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Numero Registro</t>
   </si>
@@ -30,15 +30,9 @@
     <t>Evaluador</t>
   </si>
   <si>
-    <t>Nro Evaluador</t>
-  </si>
-  <si>
     <t>Direccion</t>
   </si>
   <si>
-    <t>Nro Direccion</t>
-  </si>
-  <si>
     <t>Centro de formacion</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>Leonardo Di Caprio</t>
   </si>
   <si>
-    <t>RTC</t>
-  </si>
-  <si>
     <t>Donald Trump</t>
   </si>
   <si>
@@ -118,6 +109,9 @@
   </si>
   <si>
     <t>Chacarita</t>
+  </si>
+  <si>
+    <t>RTC1</t>
   </si>
 </sst>
 </file>
@@ -325,41 +319,45 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color theme="0" tint="-0.14999847407452621"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color theme="0" tint="-0.14999847407452621"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color theme="0" tint="-0.14999847407452621"/>
         </bottom>
         <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -699,8 +697,8 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -717,13 +715,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
@@ -740,19 +738,15 @@
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="10">
         <v>19555442</v>
@@ -761,30 +755,26 @@
         <v>24</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="3">
-        <v>123</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="3">
-        <v>18</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6">
         <v>21549639</v>
@@ -793,30 +783,26 @@
         <v>42</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="3">
-        <v>18</v>
-      </c>
-      <c r="H3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3">
-        <v>45</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="6">
         <v>53222222</v>
@@ -825,30 +811,26 @@
         <v>11</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="4">
-        <v>30</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="4">
-        <v>89</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="8">
         <v>543545363</v>
@@ -857,30 +839,26 @@
         <v>95</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="3">
-        <v>45</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="3">
-        <v>123</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6">
         <v>535262222</v>
@@ -889,30 +867,26 @@
         <v>145</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="3">
-        <v>89</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="3">
-        <v>10</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6">
         <v>42593054</v>
@@ -921,30 +895,26 @@
         <v>939</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3">
-        <v>123</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="3">
-        <v>10</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="6">
         <v>18492984</v>
@@ -953,23 +923,19 @@
         <v>404</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="3">
-        <v>10</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="3">
-        <v>18</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7"/>

</xml_diff>

<commit_message>
Retocando cosas y agregando el excel vacio para luego descargar
</commit_message>
<xml_diff>
--- a/produccion/certificadosexcel.xlsx
+++ b/produccion/certificadosexcel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Larroca\Desktop\Giuliano\ProyectoAATVAC\produccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franco\Desktop\Programacion\proyectito\GeneradorCertificadosAATVAC\produccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2238194C-F5BF-4DB7-AA2C-FDC90E8412A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -90,21 +91,12 @@
     <t>Buenos Aires</t>
   </si>
   <si>
-    <t>certificacion</t>
-  </si>
-  <si>
     <t>evaluador</t>
   </si>
   <si>
     <t>instructor</t>
   </si>
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>dni</t>
-  </si>
-  <si>
     <t>2024/26/7</t>
   </si>
   <si>
@@ -112,12 +104,21 @@
   </si>
   <si>
     <t>RTC1</t>
+  </si>
+  <si>
+    <t>Certificacion</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>DNI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -129,6 +130,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -259,29 +261,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -438,14 +445,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFF8F9FA"/>
           <bgColor rgb="FFF8F9FA"/>
         </patternFill>
@@ -461,7 +460,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Hoja1-style" pivot="0" count="2">
+    <tableStyle name="Hoja1-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="firstRowStripe" dxfId="11"/>
       <tableStyleElement type="secondRowStripe" dxfId="10"/>
     </tableStyle>
@@ -478,17 +477,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="B2:J8" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="B2:J8" headerRowCount="0">
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="8"/>
-    <tableColumn id="2" name="Column2" dataDxfId="7"/>
-    <tableColumn id="3" name="Column3" dataDxfId="6"/>
-    <tableColumn id="4" name="Column4" dataDxfId="5"/>
-    <tableColumn id="5" name="Column5" dataDxfId="4"/>
-    <tableColumn id="6" name="Column6" dataDxfId="3"/>
-    <tableColumn id="7" name="Column7" dataDxfId="2"/>
-    <tableColumn id="8" name="Column8" dataDxfId="1"/>
-    <tableColumn id="9" name="Column9" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -691,14 +690,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -706,7 +705,7 @@
     <col min="1" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" customWidth="1"/>
@@ -715,18 +714,18 @@
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -754,8 +753,8 @@
       <c r="D2" s="4">
         <v>24</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>28</v>
+      <c r="E2" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>16</v>
@@ -782,8 +781,8 @@
       <c r="D3" s="3">
         <v>42</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>28</v>
+      <c r="E3" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>17</v>
@@ -810,8 +809,8 @@
       <c r="D4" s="3">
         <v>11</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>28</v>
+      <c r="E4" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>18</v>
@@ -838,8 +837,8 @@
       <c r="D5" s="2">
         <v>95</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>28</v>
+      <c r="E5" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
@@ -855,7 +854,7 @@
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>13</v>
@@ -866,8 +865,8 @@
       <c r="D6" s="3">
         <v>145</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>28</v>
+      <c r="E6" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>20</v>
@@ -876,14 +875,14 @@
         <v>21</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>14</v>
@@ -894,8 +893,8 @@
       <c r="D7" s="3">
         <v>939</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>28</v>
+      <c r="E7" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>16</v>
@@ -911,7 +910,7 @@
     </row>
     <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>15</v>
@@ -922,8 +921,8 @@
       <c r="D8" s="3">
         <v>404</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>28</v>
+      <c r="E8" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>21</v>
@@ -940,15 +939,15 @@
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="13"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E10" s="14"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E8">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>